<commit_message>
updatedd the simple data generation procedure
</commit_message>
<xml_diff>
--- a/data/Toy 2/Generation parameters.xlsx
+++ b/data/Toy 2/Generation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/data/Toy 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{D67BAD7C-F125-4AFE-84FA-011BA22712AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A08BDA76-576D-410D-89F9-EE8F04A4E745}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{D67BAD7C-F125-4AFE-84FA-011BA22712AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54474F49-DBA2-49C6-88B4-A7CDE63CD5F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5477A2D4-2755-4465-AF13-CFA0CC252C43}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{5477A2D4-2755-4465-AF13-CFA0CC252C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,12 +88,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -451,7 +445,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>